<commit_message>
Update files in data/update_data
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_data/1907_hf_data.xlsx
+++ b/EquityHedging/data/update_data/1907_hf_data.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvg9hxp\Documents\Projects\RMP\EquityHedging\data\update_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB06E74D-820A-40A3-AE81-6B45842513B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{959A547D-FCAC-4257-8F71-2BD0D6C28CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1716" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
     <sheet name="Disclosure" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="26">
   <si>
     <t xml:space="preserve">
 Disclosure
@@ -43,7 +56,7 @@
     <t/>
   </si>
   <si>
-    <t>Data as of Friday, June 30, 2023</t>
+    <t>Data as of Thursday, November 30, 2023</t>
   </si>
   <si>
     <t>Date</t>
@@ -52,37 +65,64 @@
     <t>Account Name</t>
   </si>
   <si>
+    <t>Market Value</t>
+  </si>
+  <si>
     <t>MTD Return</t>
   </si>
   <si>
-    <t>Market Value</t>
+    <t>2023-11-30</t>
+  </si>
+  <si>
+    <t>1907 Penso Class A</t>
+  </si>
+  <si>
+    <t>1907 III Class A</t>
+  </si>
+  <si>
+    <t>1907 ARP Trend Following LLC_Class EM</t>
+  </si>
+  <si>
+    <t>1907 Kepos</t>
+  </si>
+  <si>
+    <t>1907 Systematica Trend Following</t>
+  </si>
+  <si>
+    <t>1907 III Fund Ltd _ Class CV</t>
+  </si>
+  <si>
+    <t>1907 Campbell Trend Following LLC</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-09-29</t>
+  </si>
+  <si>
+    <t>2023-08-31</t>
+  </si>
+  <si>
+    <t>2023-07-31</t>
   </si>
   <si>
     <t>2023-06-30</t>
   </si>
   <si>
-    <t>1907 III Class A</t>
-  </si>
-  <si>
-    <t>1907 ARP Trend Following LLC_Class EM</t>
-  </si>
-  <si>
-    <t>1907 Campbell Trend Following LLC</t>
-  </si>
-  <si>
-    <t>1907 Kepos</t>
-  </si>
-  <si>
-    <t>1907 Penso Class A</t>
-  </si>
-  <si>
-    <t>1907 Systematica Trend Following</t>
-  </si>
-  <si>
-    <t>1907 III Fund Ltd _ Class CV</t>
-  </si>
-  <si>
     <t>2023-05-31</t>
+  </si>
+  <si>
+    <t>2023-04-28</t>
+  </si>
+  <si>
+    <t>2023-03-31</t>
+  </si>
+  <si>
+    <t>2023-02-28</t>
+  </si>
+  <si>
+    <t>2023-01-31</t>
   </si>
 </sst>
 </file>
@@ -94,8 +134,8 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]\(#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="\$#,##0;[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="\$#,##0;[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;[Red]\(#,##0.00\)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -588,22 +628,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -617,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -631,7 +671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -645,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -659,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -667,13 +707,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="13">
-        <v>0.82</v>
+        <v>83886993.638619497</v>
       </c>
       <c r="D5" s="14">
-        <v>112554915.70282701</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>-6.63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -681,13 +721,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="13">
-        <v>2.93</v>
+        <v>80843561.282744393</v>
       </c>
       <c r="D6" s="14">
-        <v>93774466.643876806</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -695,13 +735,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="13">
-        <v>-0.51</v>
+        <v>95856883.969339401</v>
       </c>
       <c r="D7" s="14">
-        <v>190147551.05525601</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>-4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -709,13 +749,13 @@
         <v>12</v>
       </c>
       <c r="C8" s="13">
-        <v>1.67</v>
+        <v>67225700.279034898</v>
       </c>
       <c r="D8" s="14">
-        <v>177628187.43178701</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -723,13 +763,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="13">
-        <v>-1.49</v>
+        <v>219410613.83404699</v>
       </c>
       <c r="D9" s="14">
-        <v>140685590.37047699</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>-10.029999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -737,13 +777,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="13">
-        <v>-0.81</v>
+        <v>105437740.481888</v>
       </c>
       <c r="D10" s="14">
-        <v>286503825.01424003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -751,13 +791,13 @@
         <v>15</v>
       </c>
       <c r="C11" s="13">
-        <v>0.13</v>
+        <v>184510089.49280301</v>
       </c>
       <c r="D11" s="14">
-        <v>105192466.857887</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>-5.73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -771,91 +811,91 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" s="13">
-        <v>3.54</v>
+        <v>297793228.70954901</v>
       </c>
       <c r="D13" s="14">
-        <v>190828254.01556101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="13">
-        <v>-0.02</v>
+        <v>130272392.31812701</v>
       </c>
       <c r="D14" s="14">
-        <v>90841064.354998395</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C15" s="13">
-        <v>-1.78</v>
+        <v>105677969.523995</v>
       </c>
       <c r="D15" s="14">
-        <v>174350373.907695</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>-1.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16" s="13">
-        <v>0.13</v>
+        <v>105869772.17989101</v>
       </c>
       <c r="D16" s="14">
-        <v>208983227.782747</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="13">
-        <v>-3.13</v>
+        <v>100101948.403869</v>
       </c>
       <c r="D17" s="14">
-        <v>137506376.799243</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C18" s="13">
-        <v>0.84</v>
+        <v>82429721.307243496</v>
       </c>
       <c r="D18" s="14">
-        <v>288646374.335446</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -863,23 +903,1040 @@
         <v>15</v>
       </c>
       <c r="C19" s="13">
+        <v>195632858.62836701</v>
+      </c>
+      <c r="D19" s="14">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="13">
+        <v>98568466.328956902</v>
+      </c>
+      <c r="D21" s="14">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="13">
+        <v>286213393.62740201</v>
+      </c>
+      <c r="D22" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="13">
+        <v>234501779.85927999</v>
+      </c>
+      <c r="D23" s="14">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="13">
+        <v>107837309.34869801</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="13">
+        <v>132193053.41642401</v>
+      </c>
+      <c r="D25" s="14">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="13">
+        <v>192804337.25760999</v>
+      </c>
+      <c r="D26" s="14">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="13">
+        <v>79783355.5630932</v>
+      </c>
+      <c r="D27" s="14">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="13">
+        <v>181698666.18618399</v>
+      </c>
+      <c r="D29" s="14">
+        <v>-0.91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="13">
+        <v>107757758.66928799</v>
+      </c>
+      <c r="D30" s="14">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="13">
+        <v>77960479.513679206</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="13">
+        <v>188266083.98685399</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="13">
+        <v>266525362.37481099</v>
+      </c>
+      <c r="D33" s="14">
+        <v>-3.78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="13">
+        <v>95998585.593441397</v>
+      </c>
+      <c r="D34" s="14">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="13">
+        <v>128835141.601593</v>
+      </c>
+      <c r="D35" s="14">
+        <v>-1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="13">
+        <v>103626743.49211501</v>
+      </c>
+      <c r="D37" s="14">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="13">
+        <v>276383122.53143299</v>
+      </c>
+      <c r="D38" s="14">
+        <v>-3.33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="13">
+        <v>183501028.40901801</v>
+      </c>
+      <c r="D39" s="14">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="13">
+        <v>69810209.323903903</v>
+      </c>
+      <c r="D40" s="14">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="13">
+        <v>96132643.689972505</v>
+      </c>
+      <c r="D41" s="14">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="13">
+        <v>186385437.68929699</v>
+      </c>
+      <c r="D42" s="14">
+        <v>-2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="13">
+        <v>130503806.62872399</v>
+      </c>
+      <c r="D43" s="14">
+        <v>-3.62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="13">
+        <v>140689197.804546</v>
+      </c>
+      <c r="D45" s="14">
+        <v>-1.49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="13">
+        <v>286503825.01424003</v>
+      </c>
+      <c r="D46" s="14">
+        <v>-0.81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="13">
+        <v>105192466.857887</v>
+      </c>
+      <c r="D47" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="13">
+        <v>177628187.43178701</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="13">
+        <v>190147551.05525601</v>
+      </c>
+      <c r="D49" s="14">
+        <v>-0.51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="13">
+        <v>93774466.643876806</v>
+      </c>
+      <c r="D50" s="14">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="13">
+        <v>112554915.70282701</v>
+      </c>
+      <c r="D51" s="14">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="13">
+        <v>174350373.907695</v>
+      </c>
+      <c r="D53" s="14">
+        <v>-1.78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="13">
+        <v>208983227.782747</v>
+      </c>
+      <c r="D54" s="14">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="13">
+        <v>104639252.57243399</v>
+      </c>
+      <c r="D55" s="14">
         <v>0.71</v>
       </c>
-      <c r="D19" s="14">
-        <v>104639252.57243399</v>
+    </row>
+    <row r="56" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="13">
+        <v>90841064.354998395</v>
+      </c>
+      <c r="D56" s="14">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="13">
+        <v>137506376.79809701</v>
+      </c>
+      <c r="D57" s="14">
+        <v>-3.13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="13">
+        <v>288646374.335446</v>
+      </c>
+      <c r="D58" s="14">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="13">
+        <v>190828254.01556101</v>
+      </c>
+      <c r="D59" s="14">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="13">
+        <v>91116573.141908795</v>
+      </c>
+      <c r="D61" s="14">
+        <v>-1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="13">
+        <v>184310613.86393601</v>
+      </c>
+      <c r="D62" s="14">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="13">
+        <v>222068595.23519501</v>
+      </c>
+      <c r="D63" s="14">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="13">
+        <v>152363060.07925001</v>
+      </c>
+      <c r="D64" s="14">
+        <v>-3.87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="13">
+        <v>104338460.72322799</v>
+      </c>
+      <c r="D65" s="14">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="13">
+        <v>286207189.90463501</v>
+      </c>
+      <c r="D66" s="14">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="13">
+        <v>177514066.56929901</v>
+      </c>
+      <c r="D67" s="14">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="13">
+        <v>103546037.84567501</v>
+      </c>
+      <c r="D69" s="14">
+        <v>-0.78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="13">
+        <v>92360107.182299599</v>
+      </c>
+      <c r="D70" s="14">
+        <v>-0.17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="13">
+        <v>146673024.07993299</v>
+      </c>
+      <c r="D71" s="14">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="13">
+        <v>214643979.962116</v>
+      </c>
+      <c r="D72" s="14">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="13">
+        <v>178949443.485396</v>
+      </c>
+      <c r="D73" s="14">
+        <v>-4.82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="13">
+        <v>173435749.60878599</v>
+      </c>
+      <c r="D74" s="14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="13">
+        <v>282122813.26510102</v>
+      </c>
+      <c r="D75" s="14">
+        <v>-8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="13">
+        <v>104411755.336197</v>
+      </c>
+      <c r="D77" s="14">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="13">
+        <v>307263312.42034</v>
+      </c>
+      <c r="D78" s="14">
+        <v>-2.97</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="13">
+        <v>92160179.735598594</v>
+      </c>
+      <c r="D79" s="14">
+        <v>5.39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" s="13">
+        <v>246988289.36391699</v>
+      </c>
+      <c r="D80" s="14">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="13">
+        <v>188287640.05966699</v>
+      </c>
+      <c r="D81" s="14">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" s="13">
+        <v>142338831.451662</v>
+      </c>
+      <c r="D82" s="14">
+        <v>-1.66</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="13">
+        <v>214906234.63191301</v>
+      </c>
+      <c r="D83" s="14">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="13">
+        <v>87675846.672789395</v>
+      </c>
+      <c r="D85" s="14">
+        <v>-1.22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="13">
+        <v>208451354.063804</v>
+      </c>
+      <c r="D86" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="13">
+        <v>141740179.36608499</v>
+      </c>
+      <c r="D87" s="14">
+        <v>-5.0599999999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="13">
+        <v>180784705.96151</v>
+      </c>
+      <c r="D88" s="14">
+        <v>-2.41</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="13">
+        <v>242710879.35048401</v>
+      </c>
+      <c r="D89" s="14">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="13">
+        <v>316265633.22135502</v>
+      </c>
+      <c r="D90" s="14">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="13">
+        <v>104102401.639566</v>
+      </c>
+      <c r="D91" s="14">
+        <v>1.21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="13">
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A76:A83"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A60:A67"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A20:A27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:D19" numberStoredAsText="1"/>
+    <ignoredError sqref="C2:D91" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -890,17 +1947,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="3" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>